<commit_message>
add kab and kota
</commit_message>
<xml_diff>
--- a/Master Provinsi Indonesia.xlsx
+++ b/Master Provinsi Indonesia.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405"/>
@@ -28,135 +28,257 @@
     <t>Papua</t>
   </si>
   <si>
-    <t xml:space="preserve">Aceh  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sumatera Utara </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sumatera Barat  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Riau  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jambi  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sumatera Selatan  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bengkulu  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lampung  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kepulauan Bangka Belitung  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kepulauan Riau  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dki Jakarta  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jawa Barat  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jawa Tengah  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DI Yogyakarta  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jawa Timur  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Banten  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bali  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nusa Tenggara Barat  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nusa Tenggara Timur  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kalimantan Barat  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kalimantan Tengah  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kalimantan Selatan  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kalimantan Timur  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sulawesi Utara  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kalimantan Utara  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sulawesi Tengah  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sulawesi Selatan  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sulawesi Tenggara  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gorontalo  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sulawesi Barat  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maluku  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maluku Utara  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Papua Barat  </t>
+    <t>Aceh</t>
+  </si>
+  <si>
+    <t>Sumatera Utara</t>
+  </si>
+  <si>
+    <t>Sumatera Barat</t>
+  </si>
+  <si>
+    <t>Riau</t>
+  </si>
+  <si>
+    <t>Jambi</t>
+  </si>
+  <si>
+    <t>Sumatera Selatan</t>
+  </si>
+  <si>
+    <t>Bengkulu</t>
+  </si>
+  <si>
+    <t>Lampung</t>
+  </si>
+  <si>
+    <t>Kepulauan Bangka Belitung</t>
+  </si>
+  <si>
+    <t>Kepulauan Riau</t>
+  </si>
+  <si>
+    <t>Dki Jakarta</t>
+  </si>
+  <si>
+    <t>Jawa Barat</t>
+  </si>
+  <si>
+    <t>Jawa Tengah</t>
+  </si>
+  <si>
+    <t>Di Yogyakarta</t>
+  </si>
+  <si>
+    <t>Jawa Timur</t>
+  </si>
+  <si>
+    <t>Banten</t>
+  </si>
+  <si>
+    <t>Bali</t>
+  </si>
+  <si>
+    <t>Nusa Tenggara Barat</t>
+  </si>
+  <si>
+    <t>Nusa Tenggara Timur</t>
+  </si>
+  <si>
+    <t>Kalimantan Barat</t>
+  </si>
+  <si>
+    <t>Kalimantan Tengah</t>
+  </si>
+  <si>
+    <t>Kalimantan Selatan</t>
+  </si>
+  <si>
+    <t>Kalimantan Timur</t>
+  </si>
+  <si>
+    <t>Kalimantan Utara</t>
+  </si>
+  <si>
+    <t>Sulawesi Utara</t>
+  </si>
+  <si>
+    <t>Sulawesi Tengah</t>
+  </si>
+  <si>
+    <t>Sulawesi Selatan</t>
+  </si>
+  <si>
+    <t>Sulawesi Tenggara</t>
+  </si>
+  <si>
+    <t>Gorontalo</t>
+  </si>
+  <si>
+    <t>Sulawesi Barat</t>
+  </si>
+  <si>
+    <t>Maluku</t>
+  </si>
+  <si>
+    <t>Maluku Utara</t>
+  </si>
+  <si>
+    <t>Papua Barat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,8 +294,181 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -207,26 +502,221 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="32"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="32"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="43">
+    <cellStyle name="20% - Accent1" xfId="9" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="13" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="17" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="21" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="25" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="29" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="10" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="14" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="18" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="22" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="26" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="30" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="11" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="15" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="19" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="23" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="27" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="31" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="8" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="12" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="16" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="20" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="24" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="28" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="6" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text 2" xfId="41"/>
+    <cellStyle name="Good" xfId="1" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1 2" xfId="34"/>
+    <cellStyle name="Heading 2 2" xfId="35"/>
+    <cellStyle name="Heading 3 2" xfId="36"/>
+    <cellStyle name="Heading 4 2" xfId="37"/>
+    <cellStyle name="Input" xfId="4" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell 2" xfId="38"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="32"/>
+    <cellStyle name="Note 2" xfId="40"/>
+    <cellStyle name="Output" xfId="5" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title 2" xfId="33"/>
+    <cellStyle name="Total 2" xfId="42"/>
+    <cellStyle name="Warning Text 2" xfId="39"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -527,19 +1017,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="9" customWidth="1"/>
     <col min="2" max="2" width="34.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -547,318 +1037,378 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="9">
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="J2" s="6"/>
+      <c r="E2" s="10"/>
+      <c r="G2" s="11"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="9">
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="J3" s="6"/>
+      <c r="E3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="9">
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="E4" s="10"/>
+      <c r="G4" s="11"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="J5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="G5" s="11"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="9">
         <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="J6" s="6"/>
+      <c r="E6" s="10"/>
+      <c r="G6" s="11"/>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="9">
         <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="J7" s="6"/>
+      <c r="E7" s="10"/>
+      <c r="G7" s="11"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="9">
         <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="J8" s="6"/>
+      <c r="E8" s="10"/>
+      <c r="G8" s="11"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="9">
         <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="J9" s="6"/>
+      <c r="E9" s="10"/>
+      <c r="G9" s="11"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="9">
         <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="6"/>
+      <c r="E10" s="10"/>
+      <c r="G10" s="11"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="9">
         <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="6"/>
+      <c r="E11" s="10"/>
+      <c r="G11" s="11"/>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="9">
         <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="6"/>
+      <c r="E12" s="10"/>
+      <c r="G12" s="11"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="9">
         <v>32</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="6"/>
+      <c r="E13" s="10"/>
+      <c r="G13" s="11"/>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="9">
         <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="6"/>
+      <c r="E14" s="10"/>
+      <c r="G14" s="11"/>
+      <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="9">
         <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="6"/>
+      <c r="E15" s="10"/>
+      <c r="G15" s="11"/>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="9">
         <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="E16" s="10"/>
+      <c r="G16" s="11"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
         <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="G17" s="11"/>
+      <c r="J17" s="7"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="9">
         <v>51</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="6"/>
+      <c r="E18" s="10"/>
+      <c r="G18" s="11"/>
+      <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="9">
         <v>52</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="6"/>
-    </row>
-    <row r="20" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="E19" s="10"/>
+      <c r="G19" s="11"/>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
         <v>53</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J20" s="9"/>
+      <c r="E20" s="10"/>
+      <c r="G20" s="11"/>
+      <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="9">
         <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J21" s="6"/>
+      <c r="E21" s="10"/>
+      <c r="G21" s="11"/>
+      <c r="J21" s="5"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="9">
         <v>62</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J22" s="6"/>
+      <c r="E22" s="10"/>
+      <c r="G22" s="11"/>
+      <c r="J22" s="5"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="9">
         <v>63</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J23" s="6"/>
+      <c r="E23" s="10"/>
+      <c r="G23" s="11"/>
+      <c r="J23" s="5"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="9">
         <v>64</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J24" s="6"/>
-    </row>
-    <row r="25" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="E24" s="10"/>
+      <c r="G24" s="11"/>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
         <v>65</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="G25" s="11"/>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>71</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J25" s="9"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>71</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J26" s="6"/>
+      <c r="E26" s="10"/>
+      <c r="G26" s="11"/>
+      <c r="J26" s="5"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="9">
         <v>72</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J27" s="6"/>
+      <c r="E27" s="10"/>
+      <c r="G27" s="11"/>
+      <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="9">
         <v>73</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J28" s="6"/>
+      <c r="E28" s="10"/>
+      <c r="G28" s="11"/>
+      <c r="J28" s="5"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29" s="9">
         <v>74</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J29" s="6"/>
+      <c r="E29" s="10"/>
+      <c r="G29" s="11"/>
+      <c r="J29" s="5"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30" s="9">
         <v>75</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J30" s="6"/>
-    </row>
-    <row r="31" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="E30" s="10"/>
+      <c r="G30" s="11"/>
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
         <v>76</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J31" s="9"/>
+      <c r="E31" s="10"/>
+      <c r="G31" s="11"/>
+      <c r="J31" s="7"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="A32" s="9">
         <v>81</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J32" s="6"/>
-    </row>
-    <row r="33" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="E32" s="10"/>
+      <c r="G32" s="11"/>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
         <v>82</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J33" s="9"/>
+      <c r="E33" s="10"/>
+      <c r="G33" s="11"/>
+      <c r="J33" s="7"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34" s="9">
         <v>91</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J34" s="6"/>
-    </row>
-    <row r="35" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>92</v>
+      <c r="E34" s="10"/>
+      <c r="G34" s="11"/>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="9">
+        <v>94</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J35" s="9"/>
+      <c r="E35" s="10"/>
+      <c r="G35" s="11"/>
+      <c r="J35" s="7"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>